<commit_message>
Scripting DPLKKPS003-001 and DPLKINV005-001
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKEU002-001 - Keuangan - Transaksi - Keuangan Kepesertaan - Entry Penerimaan Teller Kolektif.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKEU002-001 - Keuangan - Transaksi - Keuangan Kepesertaan - Entry Penerimaan Teller Kolektif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AC771F-3145-45F4-B23E-004D784FC269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A3300C-DE57-487A-BD67-E978C2B8720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -540,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -683,6 +683,9 @@
       <c r="X2" s="7"/>
     </row>
     <row r="3" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>